<commit_message>
Validate behavior of ZIP code field.
</commit_message>
<xml_diff>
--- a/test-data/clinical-trials.xlsx
+++ b/test-data/clinical-trials.xlsx
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="91">
   <si>
     <t>Age</t>
   </si>
   <si>
-    <t>ZipCode</t>
-  </si>
-  <si>
     <t>Breast Cancer</t>
   </si>
   <si>
@@ -283,6 +280,24 @@
   </si>
   <si>
     <t>chicken</t>
+  </si>
+  <si>
+    <t>ValidZipCode</t>
+  </si>
+  <si>
+    <t>02134</t>
+  </si>
+  <si>
+    <t>20850</t>
+  </si>
+  <si>
+    <t>InvalidZipCode</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>89540</t>
   </si>
 </sst>
 </file>
@@ -392,7 +407,6 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -400,7 +414,8 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,78 +730,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
+      <c r="B3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>28</v>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="7">
+        <v>121</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="8" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="9">
-        <v>121</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -805,310 +835,310 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="10" style="6" customWidth="1"/>
-    <col min="10" max="13" width="9.140625" style="2"/>
-    <col min="14" max="14" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="2"/>
-    <col min="18" max="18" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="9.140625" style="2"/>
-    <col min="21" max="21" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="10" style="5" customWidth="1"/>
+    <col min="10" max="13" width="9.140625" style="1"/>
+    <col min="14" max="14" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="1"/>
+    <col min="18" max="18" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="9.140625" style="1"/>
+    <col min="21" max="21" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="E1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="H1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="R1" s="3" t="s">
+      <c r="N1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="S1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>75</v>
+      <c r="T1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="G2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q2" s="2" t="s">
+      <c r="N2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>76</v>
+      <c r="T2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="2" t="s">
+      <c r="G3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="R3" s="2" t="s">
+      <c r="N3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="S3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>77</v>
+      <c r="T3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="2" t="s">
+      <c r="G4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="S4" s="2" t="s">
+      <c r="N4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="T4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>78</v>
+      <c r="S4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement search by cancer  type.
</commit_message>
<xml_diff>
--- a/test-data/clinical-trials.xlsx
+++ b/test-data/clinical-trials.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSearch" sheetId="1" r:id="rId1"/>
-    <sheet name="AdvanceSearch" sheetId="2" r:id="rId2"/>
+    <sheet name="Basic Cancer Types" sheetId="3" r:id="rId2"/>
+    <sheet name="AdvanceSearch" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="101">
   <si>
     <t>Age</t>
   </si>
@@ -298,6 +299,36 @@
   </si>
   <si>
     <t>89540</t>
+  </si>
+  <si>
+    <t>Cancer Type Name</t>
+  </si>
+  <si>
+    <t>Concept ID</t>
+  </si>
+  <si>
+    <t>Adenosquamous Lung Cancer</t>
+  </si>
+  <si>
+    <t>C9133</t>
+  </si>
+  <si>
+    <t>Chronic Kidney Disease, Stage 2</t>
+  </si>
+  <si>
+    <t>C80388</t>
+  </si>
+  <si>
+    <t>Childhood Giant Cell Glioblastoma</t>
+  </si>
+  <si>
+    <t>C114966</t>
+  </si>
+  <si>
+    <t>Chronic Atrophic Gastritis</t>
+  </si>
+  <si>
+    <t>C7405</t>
   </si>
 </sst>
 </file>
@@ -732,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,6 +857,65 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W4"/>
   <sheetViews>

</xml_diff>

<commit_message>
Generic test for display of single CTS result criterion
</commit_message>
<xml_diff>
--- a/test-data/clinical-trials.xlsx
+++ b/test-data/clinical-trials.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\qa-automation\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3D1E079E-E257-4543-BD5F-57521353DF3C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSearch" sheetId="1" r:id="rId1"/>
     <sheet name="Basic Cancer Types" sheetId="3" r:id="rId2"/>
     <sheet name="AdvanceSearch" sheetId="2" r:id="rId3"/>
+    <sheet name="Criteria Display" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="109">
   <si>
     <t>Age</t>
   </si>
@@ -329,12 +331,36 @@
   </si>
   <si>
     <t>C7405</t>
+  </si>
+  <si>
+    <t>expected text</t>
+  </si>
+  <si>
+    <t>result URL</t>
+  </si>
+  <si>
+    <t>https://www-qa.cancer.gov/about-cancer/treatment/clinical-trials/search/r?q=&amp;t=&amp;a=&amp;z=20850&amp;rl=1</t>
+  </si>
+  <si>
+    <t>within 100 miles of 20850</t>
+  </si>
+  <si>
+    <t>Near ZIP Code:</t>
+  </si>
+  <si>
+    <t>Check criteria display for a ZIP code search</t>
+  </si>
+  <si>
+    <t>expected label</t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -760,7 +786,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -857,10 +883,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -916,7 +942,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView topLeftCell="O1" workbookViewId="0">
@@ -1235,4 +1261,54 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E64847-9F29-4922-AC01-652643A1CE73}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Delete no-longer available cancer type from test data.
Childhood Giant Cell Glioblastoma no longer appears in the drop-down,
making it a bit difficult to use as an affirmative test.  Oops!
</commit_message>
<xml_diff>
--- a/test-data/clinical-trials.xlsx
+++ b/test-data/clinical-trials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\qa-automation\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3D1E079E-E257-4543-BD5F-57521353DF3C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C5F1C0E3-4728-4392-8ACB-188A9F4D14EC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSearch" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="107">
   <si>
     <t>Age</t>
   </si>
@@ -319,12 +319,6 @@
   </si>
   <si>
     <t>C80388</t>
-  </si>
-  <si>
-    <t>Childhood Giant Cell Glioblastoma</t>
-  </si>
-  <si>
-    <t>C114966</t>
   </si>
   <si>
     <t>Chronic Atrophic Gastritis</t>
@@ -884,10 +878,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,14 +920,6 @@
       </c>
       <c r="B4" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1267,7 +1253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E64847-9F29-4922-AC01-652643A1CE73}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1281,30 +1267,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add criteria display test data
- Basic search ZIP [OCECTS-891]
- Basic search age [OCECTS-892]
- Basic search keyword [OCECTS-894]

Also, allow page transitions up to 20 seconds (resolves
intermittent timing issues).
</commit_message>
<xml_diff>
--- a/test-data/clinical-trials.xlsx
+++ b/test-data/clinical-trials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\qa-automation\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C5F1C0E3-4728-4392-8ACB-188A9F4D14EC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E457627E-FF07-49A0-8218-8553B4EB9E78}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSearch" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="114">
   <si>
     <t>Age</t>
   </si>
@@ -349,6 +349,27 @@
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/about-cancer/treatment/clinical-trials/search/r?q=&amp;t=&amp;a=99&amp;z=&amp;rl=1</t>
+  </si>
+  <si>
+    <t>Check criteria display for an age-based search</t>
+  </si>
+  <si>
+    <t>Age:</t>
+  </si>
+  <si>
+    <t>Check criteria display for a keyword search</t>
+  </si>
+  <si>
+    <t>Keywords/Phrases:</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/about-cancer/treatment/clinical-trials/search/r?q=chicken&amp;t=&amp;a=&amp;z=&amp;rl=1</t>
+  </si>
+  <si>
+    <t>99</t>
   </si>
 </sst>
 </file>
@@ -880,7 +901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -1251,50 +1272,82 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E64847-9F29-4922-AC01-652643A1CE73}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="9" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="9" t="s">
         <v>101</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{FA568DFE-9766-4CFC-90F5-17664655DEFD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add results page criteria display test data
* Check expanded criteria display for a search with no matches. [OCECTS-996]
* Advanced: Check criteria display for age [OCECTS-1001]
* Advanced: Check criteria display for keyword text [OCECTS-1002]
* Advanced: Check criteria display for a ZIP code search [OCECTS-1004]
* Check criteria display for VA Affairs location [OCECTS-1003]
* Check criteria display for hospital search [OCECTS-1010]
* Check criteria display for At NIH search [OCECTS-1011]
* Check criteria display for "Healthy Volunteer" search [OCECTS-1012]
* Check criteria display for Trial Type search [OCECTS-1013]
* Check criteria display for multiple trial type search [OCECTS-1014]
* Check criteria display for a single drug search [OCECTS-1015]
* Check criteria display for multiple drug search [OCECTS-1016]
* Check criteria display for a single treatment [OCECTS-1017]
* Check criteria display for multiple treatments [OCECTS-1018]
</commit_message>
<xml_diff>
--- a/test-data/clinical-trials.xlsx
+++ b/test-data/clinical-trials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\qa-automation\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E457627E-FF07-49A0-8218-8553B4EB9E78}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{135B9AB3-9858-471B-89B5-406A68807A2B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="167">
   <si>
     <t>Age</t>
   </si>
@@ -342,9 +342,6 @@
     <t>Near ZIP Code:</t>
   </si>
   <si>
-    <t>Check criteria display for a ZIP code search</t>
-  </si>
-  <si>
     <t>expected label</t>
   </si>
   <si>
@@ -354,15 +351,9 @@
     <t>https://www.cancer.gov/about-cancer/treatment/clinical-trials/search/r?q=&amp;t=&amp;a=99&amp;z=&amp;rl=1</t>
   </si>
   <si>
-    <t>Check criteria display for an age-based search</t>
-  </si>
-  <si>
     <t>Age:</t>
   </si>
   <si>
-    <t>Check criteria display for a keyword search</t>
-  </si>
-  <si>
     <t>Keywords/Phrases:</t>
   </si>
   <si>
@@ -370,6 +361,174 @@
   </si>
   <si>
     <t>99</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/about-cancer/treatment/clinical-trials/search/r?t=C2947&amp;a=&amp;q=&amp;loc=1&amp;z=96913&amp;zp=100&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>Check expanded criteria display for a search with no matches.</t>
+  </si>
+  <si>
+    <t>Primary Cancer Type/Condition:</t>
+  </si>
+  <si>
+    <t>Chordoma</t>
+  </si>
+  <si>
+    <t>Basic: Check criteria display for a ZIP code search</t>
+  </si>
+  <si>
+    <t>Basic: Check criteria display for an age-based search</t>
+  </si>
+  <si>
+    <t>Basic: Check criteria display for a keyword search</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/about-cancer/treatment/clinical-trials/search/r?t=&amp;a=25&amp;q=&amp;loc=0&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>Advanced: Check criteria display for age</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Advanced: Check criteria display for keyword text</t>
+  </si>
+  <si>
+    <t>Here's some punctuation!</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/about-cancer/treatment/clinical-trials/search/r?t=&amp;a=&amp;q=Here%27s+some+punctuation%21&amp;loc=0&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>Check criteria display for VA Affairs location</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/about-cancer/treatment/clinical-trials/search/r?t=&amp;a=&amp;q=&amp;va=1&amp;loc=0&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>Veterans Affairs Facilities:</t>
+  </si>
+  <si>
+    <t>Results limited to trials at Veterans Affairs facilities</t>
+  </si>
+  <si>
+    <t>Advanced: Check criteria display for a ZIP code search</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/about-cancer/treatment/clinical-trials/search/r?t=&amp;a=&amp;q=&amp;loc=1&amp;z=20850&amp;zp=200&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>within 200 miles of 20850</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/about-cancer/treatment/clinical-trials/search/r?t=&amp;a=&amp;q=&amp;loc=3&amp;hos=Johns+Hopkins+University+%2F+Sidney+Kimmel+Cancer+Center&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>At Hospital/Institution:</t>
+  </si>
+  <si>
+    <t>Johns Hopkins University / Sidney Kimmel Cancer Center</t>
+  </si>
+  <si>
+    <t>Check criteria display for hospital search</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/about-cancer/treatment/clinical-trials/search/r?t=&amp;a=&amp;q=&amp;loc=4&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>At NIH:</t>
+  </si>
+  <si>
+    <t>Only show trials at the NIH Clinical Center (Bethesda, MD)</t>
+  </si>
+  <si>
+    <t>Check criteria display for At NIH search</t>
+  </si>
+  <si>
+    <t>Check criteria display for "Healthy Volunteer" search</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/about-cancer/treatment/clinical-trials/search/r?t=&amp;a=&amp;q=&amp;loc=0&amp;hv=1&amp;tt=&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>Healthy Volunteers:</t>
+  </si>
+  <si>
+    <t>Results limited to trials accepting healthy volunteers</t>
+  </si>
+  <si>
+    <t>Check criteria display for Trial Type search</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/about-cancer/treatment/clinical-trials/search/r?t=&amp;a=&amp;q=&amp;loc=0&amp;tt=treatment&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>Trial Type:</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/about-cancer/treatment/clinical-trials/search/r?t=&amp;a=&amp;q=&amp;loc=0&amp;tt=treatment&amp;tt=supportive_care&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>Treatment, Supportive Care</t>
+  </si>
+  <si>
+    <t>Check criteria display for multiple trial type search</t>
+  </si>
+  <si>
+    <t>Supportive Care, Health Services Research</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/about-cancer/treatment/clinical-trials/search/r?t=&amp;a=&amp;q=&amp;loc=0&amp;tt=supportive_care&amp;tt=health_services_research&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>Check criteria display for a single drug search</t>
+  </si>
+  <si>
+    <t>Drug/Drug Family:</t>
+  </si>
+  <si>
+    <t>Bevacizumab</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/about-cancer/treatment/clinical-trials/search/r?t=&amp;a=&amp;q=&amp;loc=0&amp;tt=&amp;d=C2039&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/about-cancer/treatment/clinical-trials/search/r?t=&amp;a=&amp;q=&amp;loc=0&amp;tt=&amp;d=C2039&amp;d=C285&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>Check criteria display for multiple drug search</t>
+  </si>
+  <si>
+    <t>Bevacizumab, Ascorbic Acid</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/about-cancer/treatment/clinical-trials/search/r?t=&amp;a=&amp;q=&amp;loc=0&amp;tt=&amp;d=C2039&amp;d=C285&amp;d=C47785&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>Bevacizumab, Ascorbic Acid, Zafirlukast</t>
+  </si>
+  <si>
+    <t>Check criteria display for a single treatment</t>
+  </si>
+  <si>
+    <t>Other Treatments:</t>
+  </si>
+  <si>
+    <t>Computed Tomography</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/about-cancer/treatment/clinical-trials/search/r?t=&amp;a=&amp;q=&amp;loc=0&amp;tt=&amp;i=C17204&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
+  </si>
+  <si>
+    <t>Check criteria display for multiple treatments</t>
+  </si>
+  <si>
+    <t>Computed Tomography, Saline</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/about-cancer/treatment/clinical-trials/search/r?t=&amp;a=&amp;q=&amp;loc=0&amp;tt=&amp;i=C17204&amp;i=C821&amp;tp=&amp;tid=&amp;in=&amp;lo=&amp;rl=2</t>
   </si>
 </sst>
 </file>
@@ -477,7 +636,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -488,6 +647,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1272,10 +1432,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E64847-9F29-4922-AC01-652643A1CE73}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,10 +1449,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>99</v>
@@ -1303,7 +1463,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>103</v>
@@ -1317,30 +1477,254 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>84</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>112</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>